<commit_message>
Docs:final cleaned data and data and final one hot encoded data
</commit_message>
<xml_diff>
--- a/cleaned_data.xlsx
+++ b/cleaned_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N99"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,21 +489,6 @@
           <t>Recommended Action</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_Cleaned</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_Confidence</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_Status</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -555,19 +540,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS AND FOR HPV VACCINE</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS AND FOR HPV VACCINE</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>100</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -619,19 +591,6 @@
           <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="M3" t="n">
-        <v>100</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -683,19 +642,6 @@
           <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="M4" t="n">
-        <v>100</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -747,19 +693,6 @@
           <t>FOR HPV VACCINE, LIFESTYLE AND SEXUAL EDUCATION</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>FOR HPV VACCINE, LIFESTYLE, AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="M5" t="n">
-        <v>99</v>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -811,19 +744,6 @@
           <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>100</v>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -875,19 +795,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS AND FOR HPV VACCINE</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS AND FOR HPV VACCINE</t>
-        </is>
-      </c>
-      <c r="M7" t="n">
-        <v>100</v>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -939,19 +846,6 @@
           <t>FOR COLPOSCOPY CYTOLOGY AND BIOPSY</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M8" t="n">
-        <v>95</v>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1003,19 +897,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M9" t="n">
-        <v>100</v>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1067,19 +948,6 @@
           <t>FOR COLPOSCOPY BIOSY, CYTOLOGY+/- TAH</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, CYTOLOGY +/- TAH</t>
-        </is>
-      </c>
-      <c r="M10" t="n">
-        <v>96</v>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1131,19 +999,6 @@
           <t>FOR BIOPSY AND CYTOLOGY WITH TAH NOT RECOMMENDED</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>FOR BIOPSY AND CYTOLOGY (TAH NOT RECOMMENDED)</t>
-        </is>
-      </c>
-      <c r="M11" t="n">
-        <v>96</v>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1195,19 +1050,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M12" t="n">
-        <v>100</v>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1259,19 +1101,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M13" t="n">
-        <v>100</v>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1323,19 +1152,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M14" t="n">
-        <v>95</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1387,19 +1203,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M15" t="n">
-        <v>95</v>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1451,19 +1254,6 @@
           <t>FOR ANNUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M16" t="n">
-        <v>100</v>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1515,19 +1305,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M17" t="n">
-        <v>95</v>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1579,19 +1356,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M18" t="n">
-        <v>100</v>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1643,19 +1407,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M19" t="n">
-        <v>100</v>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1707,19 +1458,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M20" t="n">
-        <v>100</v>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1771,19 +1509,6 @@
           <t>FOR ANNUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M21" t="n">
-        <v>100</v>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1835,19 +1560,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M22" t="n">
-        <v>100</v>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1899,19 +1611,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M23" t="n">
-        <v>100</v>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1963,19 +1662,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M24" t="n">
-        <v>100</v>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2027,19 +1713,6 @@
           <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="M25" t="n">
-        <v>100</v>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2091,19 +1764,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M26" t="n">
-        <v>95</v>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2155,19 +1815,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M27" t="n">
-        <v>95</v>
-      </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2219,19 +1866,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M28" t="n">
-        <v>95</v>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2283,19 +1917,6 @@
           <t>FOR ANNUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M29" t="n">
-        <v>100</v>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2347,19 +1968,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M30" t="n">
-        <v>100</v>
-      </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2411,19 +2019,6 @@
           <t>FOR PAP SMEAR</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>FOR PAP SMEAR</t>
-        </is>
-      </c>
-      <c r="M31" t="n">
-        <v>100</v>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2475,19 +2070,6 @@
           <t>FOR ANNUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M32" t="n">
-        <v>100</v>
-      </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2539,19 +2121,6 @@
           <t>FOR PAP SMEAR</t>
         </is>
       </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>FOR PAP SMEAR</t>
-        </is>
-      </c>
-      <c r="M33" t="n">
-        <v>100</v>
-      </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2603,19 +2172,6 @@
           <t>FOR ANNUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M34" t="n">
-        <v>100</v>
-      </c>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2667,19 +2223,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M35" t="n">
-        <v>95</v>
-      </c>
-      <c r="N35" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2731,19 +2274,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M36" t="n">
-        <v>95</v>
-      </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2795,19 +2325,6 @@
           <t>FOR PAP SMEAR</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>FOR PAP SMEAR</t>
-        </is>
-      </c>
-      <c r="M37" t="n">
-        <v>100</v>
-      </c>
-      <c r="N37" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2859,19 +2376,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M38" t="n">
-        <v>95</v>
-      </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2923,19 +2427,6 @@
           <t>FOR PAP SMEAR</t>
         </is>
       </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>FOR PAP SMEAR</t>
-        </is>
-      </c>
-      <c r="M39" t="n">
-        <v>100</v>
-      </c>
-      <c r="N39" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2987,19 +2478,6 @@
           <t>FOR COLPOSCPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M40" t="n">
-        <v>91</v>
-      </c>
-      <c r="N40" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -3051,19 +2529,6 @@
           <t>FOR PAP SMEAR</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>FOR PAP SMEAR</t>
-        </is>
-      </c>
-      <c r="M41" t="n">
-        <v>100</v>
-      </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -3115,19 +2580,6 @@
           <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
         </is>
       </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="M42" t="n">
-        <v>100</v>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -3179,19 +2631,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M43" t="n">
-        <v>100</v>
-      </c>
-      <c r="N43" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3243,19 +2682,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M44" t="n">
-        <v>100</v>
-      </c>
-      <c r="N44" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3307,19 +2733,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M45" t="n">
-        <v>100</v>
-      </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3371,19 +2784,6 @@
           <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="M46" t="n">
-        <v>100</v>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -3435,19 +2835,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M47" t="n">
-        <v>100</v>
-      </c>
-      <c r="N47" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -3499,19 +2886,6 @@
           <t>REPEAT PAP SMEAR IN 3YEARS</t>
         </is>
       </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M48" t="n">
-        <v>98</v>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -3563,19 +2937,6 @@
           <t>FOR PAP SMEAR</t>
         </is>
       </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>FOR PAP SMEAR</t>
-        </is>
-      </c>
-      <c r="M49" t="n">
-        <v>100</v>
-      </c>
-      <c r="N49" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3627,19 +2988,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M50" t="n">
-        <v>95</v>
-      </c>
-      <c r="N50" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3691,19 +3039,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M51" t="n">
-        <v>100</v>
-      </c>
-      <c r="N51" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3755,19 +3090,6 @@
           <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
         </is>
       </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="M52" t="n">
-        <v>100</v>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -3819,19 +3141,6 @@
           <t>FOR PAP SMEAR</t>
         </is>
       </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>FOR PAP SMEAR</t>
-        </is>
-      </c>
-      <c r="M53" t="n">
-        <v>100</v>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -3883,19 +3192,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M54" t="n">
-        <v>100</v>
-      </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3947,19 +3243,6 @@
           <t>FOR COLPOSCOPY BIOPSY AND CYTOLOGY+/- TAH</t>
         </is>
       </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M55" t="n">
-        <v>95</v>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -4011,19 +3294,6 @@
           <t>FOR LASER THERAPY</t>
         </is>
       </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>FOR LASER THERAPY</t>
-        </is>
-      </c>
-      <c r="M56" t="n">
-        <v>100</v>
-      </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -4075,19 +3345,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M57" t="n">
-        <v>100</v>
-      </c>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -4139,19 +3396,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M58" t="n">
-        <v>100</v>
-      </c>
-      <c r="N58" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -4203,19 +3447,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M59" t="n">
-        <v>100</v>
-      </c>
-      <c r="N59" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -4267,19 +3498,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M60" t="n">
-        <v>100</v>
-      </c>
-      <c r="N60" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -4331,19 +3549,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M61" t="n">
-        <v>95</v>
-      </c>
-      <c r="N61" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4395,19 +3600,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M62" t="n">
-        <v>100</v>
-      </c>
-      <c r="N62" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -4459,19 +3651,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M63" t="n">
-        <v>100</v>
-      </c>
-      <c r="N63" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -4523,19 +3702,6 @@
           <t>FOR PAP SMEAR</t>
         </is>
       </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>FOR PAP SMEAR</t>
-        </is>
-      </c>
-      <c r="M64" t="n">
-        <v>100</v>
-      </c>
-      <c r="N64" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -4587,19 +3753,6 @@
           <t>FOR PAP SMEAR</t>
         </is>
       </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>FOR PAP SMEAR</t>
-        </is>
-      </c>
-      <c r="M65" t="n">
-        <v>100</v>
-      </c>
-      <c r="N65" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4651,19 +3804,6 @@
           <t>FOR COLPOSCOPY BIOSPY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M66" t="n">
-        <v>90</v>
-      </c>
-      <c r="N66" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -4715,19 +3855,6 @@
           <t>FOR COLPOSCOPY BIOSPY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M67" t="n">
-        <v>90</v>
-      </c>
-      <c r="N67" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -4779,19 +3906,6 @@
           <t>FOR COLPOSCOPY BIOSPY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M68" t="n">
-        <v>90</v>
-      </c>
-      <c r="N68" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -4843,19 +3957,6 @@
           <t>FOR COLPOSCOPY BIOSPY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M69" t="n">
-        <v>90</v>
-      </c>
-      <c r="N69" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -4907,19 +4008,6 @@
           <t>FOR PAP SMEAR</t>
         </is>
       </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>FOR PAP SMEAR</t>
-        </is>
-      </c>
-      <c r="M70" t="n">
-        <v>100</v>
-      </c>
-      <c r="N70" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -4971,19 +4059,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M71" t="n">
-        <v>100</v>
-      </c>
-      <c r="N71" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -5035,19 +4110,6 @@
           <t>FOR COLPOSCOPY BIOSPY, CYTOLOGY +/- TAH</t>
         </is>
       </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, CYTOLOGY +/- TAH</t>
-        </is>
-      </c>
-      <c r="M72" t="n">
-        <v>96</v>
-      </c>
-      <c r="N72" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -5099,19 +4161,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L73" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M73" t="n">
-        <v>95</v>
-      </c>
-      <c r="N73" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -5163,19 +4212,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M74" t="n">
-        <v>100</v>
-      </c>
-      <c r="N74" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -5227,19 +4263,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M75" t="n">
-        <v>95</v>
-      </c>
-      <c r="N75" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -5291,19 +4314,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L76" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M76" t="n">
-        <v>100</v>
-      </c>
-      <c r="N76" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -5355,19 +4365,6 @@
           <t>FOR HPV VACCINATION AND SEXUAL EDUCATION</t>
         </is>
       </c>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="M77" t="n">
-        <v>92</v>
-      </c>
-      <c r="N77" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -5419,19 +4416,6 @@
           <t>FOR ANUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M78" t="n">
-        <v>99</v>
-      </c>
-      <c r="N78" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -5483,19 +4467,6 @@
           <t>FOR ANUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M79" t="n">
-        <v>99</v>
-      </c>
-      <c r="N79" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -5547,19 +4518,6 @@
           <t>FOR ANUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M80" t="n">
-        <v>99</v>
-      </c>
-      <c r="N80" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -5611,19 +4569,6 @@
           <t>FOR ANUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M81" t="n">
-        <v>99</v>
-      </c>
-      <c r="N81" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -5675,19 +4620,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M82" t="n">
-        <v>100</v>
-      </c>
-      <c r="N82" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -5739,19 +4671,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M83" t="n">
-        <v>100</v>
-      </c>
-      <c r="N83" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -5803,19 +4722,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M84" t="n">
-        <v>100</v>
-      </c>
-      <c r="N84" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -5867,19 +4773,6 @@
           <t>FOR COLOSCOPY BIOSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M85" t="n">
-        <v>89</v>
-      </c>
-      <c r="N85" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -5931,19 +4824,6 @@
           <t>FOR COLOSCOPY BIOSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M86" t="n">
-        <v>89</v>
-      </c>
-      <c r="N86" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -5995,19 +4875,6 @@
           <t>FOR COLOSCOPY BIOSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M87" t="n">
-        <v>89</v>
-      </c>
-      <c r="N87" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -6059,19 +4926,6 @@
           <t>FORCOLPOSCOPY, CYTOLOGY THEN LASER THERAPY</t>
         </is>
       </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, CYTOLOGY, THEN LASER THERAPY</t>
-        </is>
-      </c>
-      <c r="M88" t="n">
-        <v>98</v>
-      </c>
-      <c r="N88" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -6123,19 +4977,6 @@
           <t>FOR ANUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M89" t="n">
-        <v>99</v>
-      </c>
-      <c r="N89" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -6187,19 +5028,6 @@
           <t>FOR COLPOSOCPY BIOPSY, CYTOLOGY WITH TAH NOT RECOMMENDED</t>
         </is>
       </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>FOR BIOPSY AND CYTOLOGY (TAH NOT RECOMMENDED)</t>
-        </is>
-      </c>
-      <c r="M90" t="n">
-        <v>90</v>
-      </c>
-      <c r="N90" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -6251,19 +5079,6 @@
           <t>FOR REPEAT HPV TESTING ANNUALLY AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>FOR REPEAT HPV TESTING ANNUALLY AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M91" t="n">
-        <v>100</v>
-      </c>
-      <c r="N91" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -6315,19 +5130,6 @@
           <t>FOR HPV VACCINATION AND SEXUAL EDUCATION</t>
         </is>
       </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>FOR HPV VACCINE AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="M92" t="n">
-        <v>92</v>
-      </c>
-      <c r="N92" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -6379,19 +5181,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M93" t="n">
-        <v>100</v>
-      </c>
-      <c r="N93" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -6443,19 +5232,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L94" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M94" t="n">
-        <v>95</v>
-      </c>
-      <c r="N94" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -6507,19 +5283,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M95" t="n">
-        <v>95</v>
-      </c>
-      <c r="N95" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -6571,19 +5334,6 @@
           <t>REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M96" t="n">
-        <v>100</v>
-      </c>
-      <c r="N96" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -6635,19 +5385,6 @@
           <t>FOR ANUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
-      <c r="L97" t="inlineStr">
-        <is>
-          <t>FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="M97" t="n">
-        <v>99</v>
-      </c>
-      <c r="N97" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -6699,19 +5436,6 @@
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
         </is>
       </c>
-      <c r="L98" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
-        </is>
-      </c>
-      <c r="M98" t="n">
-        <v>95</v>
-      </c>
-      <c r="N98" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -6761,19 +5485,6 @@
       <c r="K99" t="inlineStr">
         <is>
           <t>FOR COLPOSCOPY BIOPSY, CYTOLOGY +/-TAH</t>
-        </is>
-      </c>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>FOR COLPOSCOPY, BIOPSY, CYTOLOGY +/- TAH</t>
-        </is>
-      </c>
-      <c r="M99" t="n">
-        <v>97</v>
-      </c>
-      <c r="N99" t="inlineStr">
-        <is>
-          <t>OK</t>
         </is>
       </c>
     </row>

</xml_diff>